<commit_message>
More base tiles for corridors
</commit_message>
<xml_diff>
--- a/working/Geomorph Calcs.xlsx
+++ b/working/Geomorph Calcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\hextiles\working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE82F24F-5058-400A-BA90-1B8CE9186E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AE85BD-CBD9-448A-ABEA-789E24C86F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20760" yWindow="-15330" windowWidth="24450" windowHeight="14040" xr2:uid="{FF1B99F7-F5AF-49B6-8EDD-976A31B15329}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="59">
   <si>
     <t>width</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>hor mid 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - line</t>
+  </si>
+  <si>
+    <t>door - hor 1</t>
   </si>
 </sst>
 </file>
@@ -596,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB32B072-E607-47EF-B931-ABD117479CC6}">
-  <dimension ref="B2:AC57"/>
+  <dimension ref="B2:AC61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="M62" sqref="M62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1510,6 +1516,10 @@
         <f>O49</f>
         <v>8</v>
       </c>
+      <c r="T54">
+        <f>M54</f>
+        <v>92.5</v>
+      </c>
       <c r="X54" t="s">
         <v>53</v>
       </c>
@@ -1608,6 +1618,45 @@
       <c r="AC57">
         <f t="shared" si="12"/>
         <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="10:29" x14ac:dyDescent="0.35">
+      <c r="J60" t="s">
+        <v>58</v>
+      </c>
+      <c r="L60">
+        <f>ROUND(L15+2*L5-N60/2,3)</f>
+        <v>52.74</v>
+      </c>
+      <c r="M60">
+        <f>T49+1</f>
+        <v>10.5</v>
+      </c>
+      <c r="N60">
+        <v>20</v>
+      </c>
+      <c r="O60">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="10:29" x14ac:dyDescent="0.35">
+      <c r="J61" t="s">
+        <v>57</v>
+      </c>
+      <c r="L61">
+        <f>S49</f>
+        <v>48.305</v>
+      </c>
+      <c r="M61">
+        <f>T49+2</f>
+        <v>11.5</v>
+      </c>
+      <c r="N61">
+        <f>U51</f>
+        <v>28.87</v>
+      </c>
+      <c r="O61">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Building new master with connections
</commit_message>
<xml_diff>
--- a/working/Geomorph Calcs.xlsx
+++ b/working/Geomorph Calcs.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\hextiles\working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7DDB5B-7861-428D-A328-6EA5885261E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4135BB-FC69-4B47-9A1E-31DD0BEB5B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="170" yWindow="540" windowWidth="19180" windowHeight="9620" xr2:uid="{FF1B99F7-F5AF-49B6-8EDD-976A31B15329}"/>
+    <workbookView xWindow="1810" yWindow="490" windowWidth="17200" windowHeight="10580" xr2:uid="{FF1B99F7-F5AF-49B6-8EDD-976A31B15329}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main Geomorph" sheetId="1" r:id="rId1"/>
-    <sheet name="Geo 15mm" sheetId="2" r:id="rId2"/>
+    <sheet name="Connections" sheetId="3" r:id="rId1"/>
+    <sheet name="Main Geomorph" sheetId="1" r:id="rId2"/>
+    <sheet name="Geo 15mm" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="102">
   <si>
     <t>width</t>
   </si>
@@ -259,16 +260,101 @@
   </si>
   <si>
     <t>hor left B1.6 - bottom</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>margin</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>Factor</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>Connection points</t>
+  </si>
+  <si>
+    <t>Connections</t>
+  </si>
+  <si>
+    <t>cx 1 A</t>
+  </si>
+  <si>
+    <t>cx 1 AR</t>
+  </si>
+  <si>
+    <t>cx 1 B</t>
+  </si>
+  <si>
+    <t>cx 1 C</t>
+  </si>
+  <si>
+    <t>cx 1 CR</t>
+  </si>
+  <si>
+    <t>cx 1 BR</t>
+  </si>
+  <si>
+    <t>centre</t>
+  </si>
+  <si>
+    <t>transform mm</t>
+  </si>
+  <si>
+    <t>Extensions</t>
+  </si>
+  <si>
+    <t>ext 1 B</t>
+  </si>
+  <si>
+    <t>ext 1 A</t>
+  </si>
+  <si>
+    <t>ext 1 C</t>
+  </si>
+  <si>
+    <t>ext 1 CR</t>
+  </si>
+  <si>
+    <t>ext 1 AR</t>
+  </si>
+  <si>
+    <t>ext 1 BR</t>
+  </si>
+  <si>
+    <t>Walls - Vertical</t>
+  </si>
+  <si>
+    <t>wall 1A-4AR</t>
+  </si>
+  <si>
+    <t>wall 1AR-4A</t>
+  </si>
+  <si>
+    <t>wall 6AR-2A</t>
+  </si>
+  <si>
+    <t>wall 6A-2AR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,8 +368,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,6 +394,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -309,10 +416,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,11 +763,1298 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AA65B72-3617-498E-9A9E-6C122A9690F8}">
+  <dimension ref="A2:AD50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="11">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="8">
+        <f>D6/2</f>
+        <v>14.433756729740645</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="8">
+        <f>2*D4/SQRT(3)</f>
+        <v>28.867513459481291</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="8">
+        <f>D4/4</f>
+        <v>6.25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="8">
+        <f>2/SQRT(3)*C8</f>
+        <v>7.2168783648703227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="8">
+        <f>C8/2</f>
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="8">
+        <f>2/SQRT(3)*C10</f>
+        <v>3.6084391824351614</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15">
+        <f>ROUND(C14+2*D6,3)</f>
+        <v>62.734999999999999</v>
+      </c>
+      <c r="D15">
+        <f>D14+2*D4</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16">
+        <f>2*D4-0.5*C8</f>
+        <v>46.875</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="D17">
+        <f>D16/25.4*96</f>
+        <v>177.16535433070868</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="P19" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5">
+        <v>1</v>
+      </c>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5">
+        <v>2</v>
+      </c>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5">
+        <v>3</v>
+      </c>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" t="s">
+        <v>12</v>
+      </c>
+      <c r="I20" t="s">
+        <v>24</v>
+      </c>
+      <c r="K20" t="s">
+        <v>74</v>
+      </c>
+      <c r="M20" t="s">
+        <v>75</v>
+      </c>
+      <c r="P20" t="s">
+        <v>79</v>
+      </c>
+      <c r="R20" t="s">
+        <v>13</v>
+      </c>
+      <c r="T20" t="s">
+        <v>12</v>
+      </c>
+      <c r="V20" t="s">
+        <v>24</v>
+      </c>
+      <c r="X20" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I21" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K21" t="s">
+        <v>7</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M21" t="s">
+        <v>7</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P21" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="R21" t="s">
+        <v>7</v>
+      </c>
+      <c r="S21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="T21" t="s">
+        <v>7</v>
+      </c>
+      <c r="U21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V21" t="s">
+        <v>7</v>
+      </c>
+      <c r="W21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="X21" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD21" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="8">
+        <f>$C$14+P22*$D$6</f>
+        <v>33.867513459481287</v>
+      </c>
+      <c r="D22" s="9">
+        <f>$D$14+Q22*$D$4</f>
+        <v>5</v>
+      </c>
+      <c r="E22" s="8">
+        <f>$C$14+R22*$D$6</f>
+        <v>41.084391824351613</v>
+      </c>
+      <c r="F22" s="9">
+        <f>$D$14+S22*$D$4</f>
+        <v>5</v>
+      </c>
+      <c r="G22" s="8">
+        <f>$C$14+T22*$D$6</f>
+        <v>48.301270189221938</v>
+      </c>
+      <c r="H22" s="9">
+        <f>$D$14+U22*$D$4</f>
+        <v>5</v>
+      </c>
+      <c r="I22" s="8">
+        <f>$C$14+V22*$D$6</f>
+        <v>62.735026918962582</v>
+      </c>
+      <c r="J22" s="9">
+        <f>$D$14+W22*$D$4</f>
+        <v>5</v>
+      </c>
+      <c r="K22" s="8">
+        <f>$C$14+X22*$D$6</f>
+        <v>77.168783648703226</v>
+      </c>
+      <c r="L22" s="9">
+        <f>$D$14+Y22*$D$4</f>
+        <v>5</v>
+      </c>
+      <c r="M22" s="8">
+        <f>$C$14+Z22*$D$6</f>
+        <v>84.385662013573551</v>
+      </c>
+      <c r="N22" s="9">
+        <f>$D$14+AA22*$D$4</f>
+        <v>5</v>
+      </c>
+      <c r="P22" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="6">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <f>$P22+P$19*$AC22</f>
+        <v>1.25</v>
+      </c>
+      <c r="S22" s="3">
+        <f>$Q22+P$19*$AD22</f>
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <f>$P22+R$19*$AC22</f>
+        <v>1.5</v>
+      </c>
+      <c r="U22" s="3">
+        <f>$Q22+R$19*$AD22</f>
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <f>$P22+T$19*$AC22</f>
+        <v>2</v>
+      </c>
+      <c r="W22" s="3">
+        <f>$Q22+T$19*$AD22</f>
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <f>$P22+V$19*$AC22</f>
+        <v>2.5</v>
+      </c>
+      <c r="Y22" s="3">
+        <f>$Q22+V$19*$AD22</f>
+        <v>0</v>
+      </c>
+      <c r="Z22">
+        <f>$P22+X$19*$AC22</f>
+        <v>2.75</v>
+      </c>
+      <c r="AA22" s="3">
+        <f>$Q22+X$19*$AD22</f>
+        <v>0</v>
+      </c>
+      <c r="AC22" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AD22" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="C23" s="8">
+        <f>$C$14+P23*$D$6</f>
+        <v>91.602540378443877</v>
+      </c>
+      <c r="D23" s="9">
+        <f t="shared" ref="D23:D27" si="0">$D$14+Q23*$D$4</f>
+        <v>5</v>
+      </c>
+      <c r="E23" s="8">
+        <f>$C$14+R23*$D$6</f>
+        <v>95.210979560879039</v>
+      </c>
+      <c r="F23" s="9">
+        <f t="shared" ref="F23:F27" si="1">$D$14+S23*$D$4</f>
+        <v>11.25</v>
+      </c>
+      <c r="G23" s="8">
+        <f>$C$14+T23*$D$6</f>
+        <v>98.819418743314202</v>
+      </c>
+      <c r="H23" s="9">
+        <f t="shared" ref="H23:H27" si="2">$D$14+U23*$D$4</f>
+        <v>17.5</v>
+      </c>
+      <c r="I23" s="8">
+        <f>$C$14+V23*$D$6</f>
+        <v>106.03629710818451</v>
+      </c>
+      <c r="J23" s="9">
+        <f t="shared" ref="J23:J27" si="3">$D$14+W23*$D$4</f>
+        <v>30</v>
+      </c>
+      <c r="K23" s="8">
+        <f>$C$14+X23*$D$6</f>
+        <v>113.25317547305484</v>
+      </c>
+      <c r="L23" s="9">
+        <f t="shared" ref="L23:L27" si="4">$D$14+Y23*$D$4</f>
+        <v>42.5</v>
+      </c>
+      <c r="M23" s="8">
+        <f>$C$14+Z23*$D$6</f>
+        <v>116.86161465549</v>
+      </c>
+      <c r="N23" s="9">
+        <f t="shared" ref="N23:N27" si="5">$D$14+AA23*$D$4</f>
+        <v>48.75</v>
+      </c>
+      <c r="P23" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q23" s="6">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <f>$P23+P$19*$AC23</f>
+        <v>3.125</v>
+      </c>
+      <c r="S23" s="3">
+        <f>$Q23+P$19*$AD23</f>
+        <v>0.25</v>
+      </c>
+      <c r="T23">
+        <f>$P23+R$19*$AC23</f>
+        <v>3.25</v>
+      </c>
+      <c r="U23" s="3">
+        <f>$Q23+R$19*$AD23</f>
+        <v>0.5</v>
+      </c>
+      <c r="V23">
+        <f>$P23+T$19*$AC23</f>
+        <v>3.5</v>
+      </c>
+      <c r="W23" s="3">
+        <f>$Q23+T$19*$AD23</f>
+        <v>1</v>
+      </c>
+      <c r="X23">
+        <f>$P23+V$19*$AC23</f>
+        <v>3.75</v>
+      </c>
+      <c r="Y23" s="3">
+        <f>$Q23+V$19*$AD23</f>
+        <v>1.5</v>
+      </c>
+      <c r="Z23">
+        <f>$P23+X$19*$AC23</f>
+        <v>3.875</v>
+      </c>
+      <c r="AA23" s="3">
+        <f>$Q23+X$19*$AD23</f>
+        <v>1.75</v>
+      </c>
+      <c r="AC23" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="AD23" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="C24" s="8">
+        <f>$C$14+P24*$D$6</f>
+        <v>120.47005383792516</v>
+      </c>
+      <c r="D24" s="9">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="E24" s="8">
+        <f>$C$14+R24*$D$6</f>
+        <v>116.86161465549</v>
+      </c>
+      <c r="F24" s="9">
+        <f t="shared" si="1"/>
+        <v>61.25</v>
+      </c>
+      <c r="G24" s="8">
+        <f>$C$14+T24*$D$6</f>
+        <v>113.25317547305484</v>
+      </c>
+      <c r="H24" s="9">
+        <f t="shared" si="2"/>
+        <v>67.5</v>
+      </c>
+      <c r="I24" s="8">
+        <f>$C$14+V24*$D$6</f>
+        <v>106.03629710818451</v>
+      </c>
+      <c r="J24" s="9">
+        <f t="shared" si="3"/>
+        <v>80</v>
+      </c>
+      <c r="K24" s="8">
+        <f>$C$14+X24*$D$6</f>
+        <v>98.819418743314202</v>
+      </c>
+      <c r="L24" s="9">
+        <f t="shared" si="4"/>
+        <v>92.5</v>
+      </c>
+      <c r="M24" s="8">
+        <f>$C$14+Z24*$D$6</f>
+        <v>95.210979560879039</v>
+      </c>
+      <c r="N24" s="9">
+        <f t="shared" si="5"/>
+        <v>98.75</v>
+      </c>
+      <c r="P24" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q24" s="6">
+        <v>2</v>
+      </c>
+      <c r="R24">
+        <f>$P24+P$19*$AC24</f>
+        <v>3.875</v>
+      </c>
+      <c r="S24" s="3">
+        <f>$Q24+P$19*$AD24</f>
+        <v>2.25</v>
+      </c>
+      <c r="T24">
+        <f>$P24+R$19*$AC24</f>
+        <v>3.75</v>
+      </c>
+      <c r="U24" s="3">
+        <f>$Q24+R$19*$AD24</f>
+        <v>2.5</v>
+      </c>
+      <c r="V24">
+        <f>$P24+T$19*$AC24</f>
+        <v>3.5</v>
+      </c>
+      <c r="W24" s="3">
+        <f>$Q24+T$19*$AD24</f>
+        <v>3</v>
+      </c>
+      <c r="X24">
+        <f>$P24+V$19*$AC24</f>
+        <v>3.25</v>
+      </c>
+      <c r="Y24" s="3">
+        <f>$Q24+V$19*$AD24</f>
+        <v>3.5</v>
+      </c>
+      <c r="Z24">
+        <f>$P24+X$19*$AC24</f>
+        <v>3.125</v>
+      </c>
+      <c r="AA24" s="3">
+        <f>$Q24+X$19*$AD24</f>
+        <v>3.75</v>
+      </c>
+      <c r="AC24" s="5">
+        <v>-0.25</v>
+      </c>
+      <c r="AD24" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="C25" s="8">
+        <f>$C$14+P25*$D$6</f>
+        <v>91.602540378443877</v>
+      </c>
+      <c r="D25" s="9">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="E25" s="8">
+        <f>$C$14+R25*$D$6</f>
+        <v>84.385662013573551</v>
+      </c>
+      <c r="F25" s="9">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="G25" s="8">
+        <f>$C$14+T25*$D$6</f>
+        <v>77.168783648703226</v>
+      </c>
+      <c r="H25" s="9">
+        <f t="shared" si="2"/>
+        <v>105</v>
+      </c>
+      <c r="I25" s="8">
+        <f>$C$14+V25*$D$6</f>
+        <v>62.735026918962582</v>
+      </c>
+      <c r="J25" s="9">
+        <f t="shared" si="3"/>
+        <v>105</v>
+      </c>
+      <c r="K25" s="8">
+        <f>$C$14+X25*$D$6</f>
+        <v>48.301270189221938</v>
+      </c>
+      <c r="L25" s="9">
+        <f t="shared" si="4"/>
+        <v>105</v>
+      </c>
+      <c r="M25" s="8">
+        <f>$C$14+Z25*$D$6</f>
+        <v>41.084391824351613</v>
+      </c>
+      <c r="N25" s="9">
+        <f t="shared" si="5"/>
+        <v>105</v>
+      </c>
+      <c r="P25" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q25" s="6">
+        <v>4</v>
+      </c>
+      <c r="R25">
+        <f>$P25+P$19*$AC25</f>
+        <v>2.75</v>
+      </c>
+      <c r="S25" s="3">
+        <f>$Q25+P$19*$AD25</f>
+        <v>4</v>
+      </c>
+      <c r="T25">
+        <f>$P25+R$19*$AC25</f>
+        <v>2.5</v>
+      </c>
+      <c r="U25" s="3">
+        <f>$Q25+R$19*$AD25</f>
+        <v>4</v>
+      </c>
+      <c r="V25">
+        <f>$P25+T$19*$AC25</f>
+        <v>2</v>
+      </c>
+      <c r="W25" s="3">
+        <f>$Q25+T$19*$AD25</f>
+        <v>4</v>
+      </c>
+      <c r="X25">
+        <f>$P25+V$19*$AC25</f>
+        <v>1.5</v>
+      </c>
+      <c r="Y25" s="3">
+        <f>$Q25+V$19*$AD25</f>
+        <v>4</v>
+      </c>
+      <c r="Z25">
+        <f>$P25+X$19*$AC25</f>
+        <v>1.25</v>
+      </c>
+      <c r="AA25" s="3">
+        <f>$Q25+X$19*$AD25</f>
+        <v>4</v>
+      </c>
+      <c r="AC25" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="AD25" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="C26" s="8">
+        <f>$C$14+P26*$D$6</f>
+        <v>33.867513459481287</v>
+      </c>
+      <c r="D26" s="9">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="E26" s="8">
+        <f>$C$14+R26*$D$6</f>
+        <v>30.259074277046128</v>
+      </c>
+      <c r="F26" s="9">
+        <f t="shared" si="1"/>
+        <v>98.75</v>
+      </c>
+      <c r="G26" s="8">
+        <f>$C$14+T26*$D$6</f>
+        <v>26.650635094610969</v>
+      </c>
+      <c r="H26" s="9">
+        <f t="shared" si="2"/>
+        <v>92.5</v>
+      </c>
+      <c r="I26" s="8">
+        <f>$C$14+V26*$D$6</f>
+        <v>19.433756729740644</v>
+      </c>
+      <c r="J26" s="9">
+        <f t="shared" si="3"/>
+        <v>80</v>
+      </c>
+      <c r="K26" s="8">
+        <f>$C$14+X26*$D$6</f>
+        <v>12.216878364870322</v>
+      </c>
+      <c r="L26" s="9">
+        <f t="shared" si="4"/>
+        <v>67.5</v>
+      </c>
+      <c r="M26" s="8">
+        <f>$C$14+Z26*$D$6</f>
+        <v>8.6084391824351609</v>
+      </c>
+      <c r="N26" s="9">
+        <f t="shared" si="5"/>
+        <v>61.25</v>
+      </c>
+      <c r="P26" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="6">
+        <v>4</v>
+      </c>
+      <c r="R26">
+        <f>$P26+P$19*$AC26</f>
+        <v>0.875</v>
+      </c>
+      <c r="S26" s="3">
+        <f>$Q26+P$19*$AD26</f>
+        <v>3.75</v>
+      </c>
+      <c r="T26">
+        <f>$P26+R$19*$AC26</f>
+        <v>0.75</v>
+      </c>
+      <c r="U26" s="3">
+        <f>$Q26+R$19*$AD26</f>
+        <v>3.5</v>
+      </c>
+      <c r="V26">
+        <f>$P26+T$19*$AC26</f>
+        <v>0.5</v>
+      </c>
+      <c r="W26" s="3">
+        <f>$Q26+T$19*$AD26</f>
+        <v>3</v>
+      </c>
+      <c r="X26">
+        <f>$P26+V$19*$AC26</f>
+        <v>0.25</v>
+      </c>
+      <c r="Y26" s="3">
+        <f>$Q26+V$19*$AD26</f>
+        <v>2.5</v>
+      </c>
+      <c r="Z26">
+        <f>$P26+X$19*$AC26</f>
+        <v>0.125</v>
+      </c>
+      <c r="AA26" s="3">
+        <f>$Q26+X$19*$AD26</f>
+        <v>2.25</v>
+      </c>
+      <c r="AC26" s="5">
+        <v>-0.25</v>
+      </c>
+      <c r="AD26" s="6">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="C27" s="8">
+        <f>$C$14+P27*$D$6</f>
+        <v>5</v>
+      </c>
+      <c r="D27" s="9">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="E27" s="8">
+        <f>$C$14+R27*$D$6</f>
+        <v>8.6084391824351609</v>
+      </c>
+      <c r="F27" s="9">
+        <f t="shared" si="1"/>
+        <v>48.75</v>
+      </c>
+      <c r="G27" s="8">
+        <f>$C$14+T27*$D$6</f>
+        <v>12.216878364870322</v>
+      </c>
+      <c r="H27" s="9">
+        <f t="shared" si="2"/>
+        <v>42.5</v>
+      </c>
+      <c r="I27" s="8">
+        <f>$C$14+V27*$D$6</f>
+        <v>19.433756729740644</v>
+      </c>
+      <c r="J27" s="9">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="K27" s="8">
+        <f>$C$14+X27*$D$6</f>
+        <v>26.650635094610969</v>
+      </c>
+      <c r="L27" s="9">
+        <f t="shared" si="4"/>
+        <v>17.5</v>
+      </c>
+      <c r="M27" s="8">
+        <f>$C$14+Z27*$D$6</f>
+        <v>30.259074277046128</v>
+      </c>
+      <c r="N27" s="9">
+        <f t="shared" si="5"/>
+        <v>11.25</v>
+      </c>
+      <c r="P27" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="6">
+        <v>2</v>
+      </c>
+      <c r="R27">
+        <f>$P27+P$19*$AC27</f>
+        <v>0.125</v>
+      </c>
+      <c r="S27" s="3">
+        <f>$Q27+P$19*$AD27</f>
+        <v>1.75</v>
+      </c>
+      <c r="T27">
+        <f>$P27+R$19*$AC27</f>
+        <v>0.25</v>
+      </c>
+      <c r="U27" s="3">
+        <f>$Q27+R$19*$AD27</f>
+        <v>1.5</v>
+      </c>
+      <c r="V27">
+        <f>$P27+T$19*$AC27</f>
+        <v>0.5</v>
+      </c>
+      <c r="W27" s="3">
+        <f>$Q27+T$19*$AD27</f>
+        <v>1</v>
+      </c>
+      <c r="X27">
+        <f>$P27+V$19*$AC27</f>
+        <v>0.75</v>
+      </c>
+      <c r="Y27" s="3">
+        <f>$Q27+V$19*$AD27</f>
+        <v>0.5</v>
+      </c>
+      <c r="Z27">
+        <f>$P27+X$19*$AC27</f>
+        <v>0.875</v>
+      </c>
+      <c r="AA27" s="3">
+        <f>$Q27+X$19*$AD27</f>
+        <v>0.25</v>
+      </c>
+      <c r="AC27" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="AD27" s="6">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="2">
+        <f>ROUND(E$22-$C$9,3)</f>
+        <v>33.868000000000002</v>
+      </c>
+      <c r="D31">
+        <f>D22</f>
+        <v>5</v>
+      </c>
+      <c r="E31" s="2">
+        <f>ROUND(C9,3)</f>
+        <v>7.2169999999999996</v>
+      </c>
+      <c r="F31">
+        <f>C8</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="2">
+        <f>ROUND(G$22-$C$9,3)</f>
+        <v>41.084000000000003</v>
+      </c>
+      <c r="D32">
+        <f>D$31</f>
+        <v>5</v>
+      </c>
+      <c r="E32">
+        <f t="shared" ref="E32:F36" si="6">E$31</f>
+        <v>7.2169999999999996</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="6"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="2">
+        <f>ROUND(I$22-$C$9,3)</f>
+        <v>55.518000000000001</v>
+      </c>
+      <c r="D33">
+        <f t="shared" ref="D33:F36" si="7">D$31</f>
+        <v>5</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="6"/>
+        <v>7.2169999999999996</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="6"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="2">
+        <f>ROUND(I$22,3)</f>
+        <v>62.734999999999999</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="6"/>
+        <v>7.2169999999999996</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="6"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="2">
+        <f>ROUND(K$22,3)</f>
+        <v>77.168999999999997</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="6"/>
+        <v>7.2169999999999996</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="6"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="2">
+        <f>ROUND(M$22,3)</f>
+        <v>84.385999999999996</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="6"/>
+        <v>7.2169999999999996</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="6"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="2">
+        <f>C22</f>
+        <v>33.867513459481287</v>
+      </c>
+      <c r="D39" s="12">
+        <f>D22</f>
+        <v>5</v>
+      </c>
+      <c r="E39" s="2">
+        <f>ROUND(1/8*$D$6,3)</f>
+        <v>3.6080000000000001</v>
+      </c>
+      <c r="F39" s="10">
+        <f>C8</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="2">
+        <f>C39</f>
+        <v>33.867513459481287</v>
+      </c>
+      <c r="D40">
+        <f>D$31</f>
+        <v>5</v>
+      </c>
+      <c r="E40">
+        <f>ROUND(3/8*$D$6,3)</f>
+        <v>10.824999999999999</v>
+      </c>
+      <c r="F40">
+        <f t="shared" ref="E40:F44" si="8">F$31</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="2">
+        <f>ROUND(I$22-$C$9,3)</f>
+        <v>55.518000000000001</v>
+      </c>
+      <c r="D41">
+        <f t="shared" ref="D41:F44" si="9">D$31</f>
+        <v>5</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="8"/>
+        <v>7.2169999999999996</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="8"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="2">
+        <f>ROUND(I$22,3)</f>
+        <v>62.734999999999999</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="8"/>
+        <v>7.2169999999999996</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="8"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="2">
+        <f>ROUND(K$22+1/8*D6,3)</f>
+        <v>80.777000000000001</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="E43">
+        <f>E40</f>
+        <v>10.824999999999999</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="8"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="2">
+        <f>ROUND(M$22,3)</f>
+        <v>84.385999999999996</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="8"/>
+        <v>7.2169999999999996</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="8"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" s="2">
+        <f>C32</f>
+        <v>41.084000000000003</v>
+      </c>
+      <c r="D47" s="2">
+        <f>D32</f>
+        <v>5</v>
+      </c>
+      <c r="E47" s="2">
+        <f>E32</f>
+        <v>7.2169999999999996</v>
+      </c>
+      <c r="F47">
+        <f>4*$D$4</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48" s="2">
+        <f>C35</f>
+        <v>77.168999999999997</v>
+      </c>
+      <c r="D48" s="2">
+        <f>D35</f>
+        <v>5</v>
+      </c>
+      <c r="E48" s="2">
+        <f>E35</f>
+        <v>7.2169999999999996</v>
+      </c>
+      <c r="F48">
+        <f>4*$D$4</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>100</v>
+      </c>
+      <c r="C49" s="8">
+        <f>ROUND($K$27+1/8*$D$6,3)</f>
+        <v>30.259</v>
+      </c>
+      <c r="D49" s="8">
+        <f>$L$27-$C$8</f>
+        <v>11.25</v>
+      </c>
+      <c r="E49">
+        <f>ROUND(2.25*$D$6,3)</f>
+        <v>64.951999999999998</v>
+      </c>
+      <c r="F49" s="8">
+        <f>C8</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50" s="8">
+        <f>ROUND($G$27,3)</f>
+        <v>12.217000000000001</v>
+      </c>
+      <c r="D50" s="8">
+        <f>H27</f>
+        <v>42.5</v>
+      </c>
+      <c r="E50">
+        <f>ROUND(3.5*$D$6,3)</f>
+        <v>101.036</v>
+      </c>
+      <c r="F50" s="8">
+        <f>F49</f>
+        <v>6.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB32B072-E607-47EF-B931-ABD117479CC6}">
   <dimension ref="B2:AC79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K47" workbookViewId="0">
-      <selection activeCell="S59" sqref="S59"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2018,7 +3422,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7659A5BC-8263-4306-A02D-42C7263AD0FC}">
   <dimension ref="B2:U27"/>
   <sheetViews>

</xml_diff>

<commit_message>
Colour in round areas
</commit_message>
<xml_diff>
--- a/working/Geomorph Calcs.xlsx
+++ b/working/Geomorph Calcs.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\hextiles\working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC307E91-0BA0-41FF-994C-E63AEC738E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D65BC91-591D-4C18-B72F-F2F7EC202628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20385" yWindow="-15435" windowWidth="27660" windowHeight="14715" xr2:uid="{FF1B99F7-F5AF-49B6-8EDD-976A31B15329}"/>
+    <workbookView xWindow="21480" yWindow="-14625" windowWidth="21600" windowHeight="11595" xr2:uid="{FF1B99F7-F5AF-49B6-8EDD-976A31B15329}"/>
   </bookViews>
   <sheets>
     <sheet name="Connections" sheetId="3" r:id="rId1"/>
-    <sheet name="Main Geomorph" sheetId="1" r:id="rId2"/>
-    <sheet name="Geo 15mm" sheetId="2" r:id="rId3"/>
+    <sheet name="Bricks" sheetId="4" r:id="rId2"/>
+    <sheet name="Main Geomorph" sheetId="1" r:id="rId3"/>
+    <sheet name="Geo 15mm" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="154">
   <si>
     <t>width</t>
   </si>
@@ -361,12 +362,6 @@
     <t>With connection points, e.g. A, there are 6 vertical pairs and 4 horizontal pairs</t>
   </si>
   <si>
-    <t>wall hor A-i part3</t>
-  </si>
-  <si>
-    <t>wall hor A-ii part3</t>
-  </si>
-  <si>
     <t>Walls - Horizontals</t>
   </si>
   <si>
@@ -376,9 +371,6 @@
     <t>wall ver A-iv part3-5</t>
   </si>
   <si>
-    <t>wall hor A-iii part1</t>
-  </si>
-  <si>
     <t>wall hor A-iv part1</t>
   </si>
   <si>
@@ -386,6 +378,129 @@
   </si>
   <si>
     <t>wall ver A-iii part5</t>
+  </si>
+  <si>
+    <t>wall hor A-i part4</t>
+  </si>
+  <si>
+    <t>wall hor A-ii part4</t>
+  </si>
+  <si>
+    <t>wall hor A-iii part1-2</t>
+  </si>
+  <si>
+    <t>wall hor C-i part4</t>
+  </si>
+  <si>
+    <t>wall hor C-iv part4</t>
+  </si>
+  <si>
+    <t>wall hor C-iv part3</t>
+  </si>
+  <si>
+    <t>circle pass</t>
+  </si>
+  <si>
+    <t>wall hor C-i part4 round</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>corner radius</t>
+  </si>
+  <si>
+    <t>approx 1mm</t>
+  </si>
+  <si>
+    <t>tiled clones</t>
+  </si>
+  <si>
+    <t>rows</t>
+  </si>
+  <si>
+    <t>cols</t>
+  </si>
+  <si>
+    <t>shift</t>
+  </si>
+  <si>
+    <t>row</t>
+  </si>
+  <si>
+    <t>col</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>storke</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>solid</t>
+  </si>
+  <si>
+    <t>fill</t>
+  </si>
+  <si>
+    <t>? (undefined) - so it can be replaced</t>
+  </si>
+  <si>
+    <t>colour</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>rand</t>
+  </si>
+  <si>
+    <t>H50 S10 L50</t>
+  </si>
+  <si>
+    <t>initial</t>
+  </si>
+  <si>
+    <t>Edit &gt; Clone &gt; Unlink Clone</t>
+  </si>
+  <si>
+    <t>Move the original out of the way</t>
+  </si>
+  <si>
+    <t>Select all</t>
+  </si>
+  <si>
+    <t>Extensions &gt; Modify Path &gt; Fractalise</t>
+  </si>
+  <si>
+    <t>Subdivisions</t>
+  </si>
+  <si>
+    <t>Smoothness</t>
+  </si>
+  <si>
+    <t>Node Tool</t>
+  </si>
+  <si>
+    <t>Select all nodes</t>
+  </si>
+  <si>
+    <t>Make selected nodes smooth</t>
+  </si>
+  <si>
+    <t>wall ver A-iii part5 round</t>
+  </si>
+  <si>
+    <t>wall hor A-iv part4 round</t>
   </si>
 </sst>
 </file>
@@ -396,7 +511,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -421,6 +536,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -458,7 +589,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -471,6 +602,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -805,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AA65B72-3617-498E-9A9E-6C122A9690F8}">
-  <dimension ref="A2:AD65"/>
+  <dimension ref="A2:AD73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -816,12 +950,12 @@
     <col min="1" max="1" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -832,7 +966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -844,7 +978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -856,10 +990,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -871,7 +1005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -880,7 +1014,7 @@
         <v>7.2168783648703227</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -889,7 +1023,7 @@
         <v>3.125</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -898,7 +1032,7 @@
         <v>3.6084391824351614</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>7</v>
       </c>
@@ -906,7 +1040,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -917,7 +1051,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>88</v>
       </c>
@@ -930,13 +1064,20 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>89</v>
       </c>
       <c r="D16">
         <f>2*D4-0.5*C8</f>
         <v>46.875</v>
+      </c>
+      <c r="E16" t="s">
+        <v>119</v>
+      </c>
+      <c r="F16">
+        <f>2*D4-0.5*15</f>
+        <v>42.5</v>
       </c>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.35">
@@ -944,6 +1085,10 @@
         <f>D16/25.4*96</f>
         <v>177.16535433070868</v>
       </c>
+      <c r="F17">
+        <f>F16/25.4*96</f>
+        <v>160.62992125984255</v>
+      </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
@@ -2064,7 +2209,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C52" s="2">
         <f>C49</f>
@@ -2085,14 +2230,14 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C53" s="2">
         <f>C52</f>
         <v>41.084000000000003</v>
       </c>
       <c r="D53" s="2">
-        <f>D65</f>
+        <f>D66</f>
         <v>92.5</v>
       </c>
       <c r="E53" s="2">
@@ -2106,7 +2251,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C54" s="2">
         <f>C50</f>
@@ -2127,14 +2272,14 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C55" s="2">
         <f>C54</f>
         <v>77.168999999999997</v>
       </c>
       <c r="D55" s="2">
-        <f>D60</f>
+        <f>D61</f>
         <v>42.5</v>
       </c>
       <c r="E55" s="2">
@@ -2152,102 +2297,101 @@
       <c r="E56" s="2"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
+      <c r="A57" t="s">
+        <v>152</v>
+      </c>
+      <c r="C57" s="2">
+        <f>C53</f>
+        <v>41.084000000000003</v>
+      </c>
+      <c r="D57" s="2">
+        <f>4*D4+D14-F57</f>
+        <v>91.6</v>
+      </c>
+      <c r="E57" s="2">
+        <f>E53</f>
+        <v>7.2169999999999996</v>
+      </c>
+      <c r="F57" s="5">
+        <v>13.4</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>109</v>
-      </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
+        <v>107</v>
+      </c>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>100</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>102</v>
       </c>
-      <c r="C59" s="7">
+      <c r="C60" s="7">
         <f>ROUND($K$27+1/8*$D$6,3)</f>
         <v>30.259</v>
       </c>
-      <c r="D59" s="7">
+      <c r="D60" s="7">
         <f>$L$27-$C$8</f>
         <v>11.25</v>
       </c>
-      <c r="E59">
+      <c r="E60">
         <f>ROUND(2.25*$D$6,3)</f>
         <v>64.951999999999998</v>
       </c>
-      <c r="F59" s="7">
+      <c r="F60" s="7">
         <f>C8</f>
         <v>6.25</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>101</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>103</v>
       </c>
-      <c r="C60" s="7">
+      <c r="C61" s="7">
         <f>ROUND($G$27,3)</f>
         <v>12.217000000000001</v>
       </c>
-      <c r="D60" s="7">
+      <c r="D61" s="7">
         <f>H27</f>
         <v>42.5</v>
       </c>
-      <c r="E60">
+      <c r="E61">
         <f>ROUND(3.5*$D$6,3)</f>
         <v>101.036</v>
       </c>
-      <c r="F60" s="7">
-        <f>F59</f>
+      <c r="F61" s="7">
+        <f>F60</f>
         <v>6.25</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>107</v>
-      </c>
-      <c r="C62" s="2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>113</v>
+      </c>
+      <c r="C63" s="2">
         <f>C50</f>
         <v>77.168999999999997</v>
       </c>
-      <c r="D62" s="7">
-        <f>D59</f>
-        <v>11.25</v>
-      </c>
-      <c r="E62" s="7">
-        <f>E59+C59-C62</f>
-        <v>18.042000000000002</v>
-      </c>
-      <c r="F62" s="7">
-        <f>F59</f>
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>108</v>
-      </c>
-      <c r="C63" s="2">
-        <f>C62</f>
-        <v>77.168999999999997</v>
-      </c>
       <c r="D63" s="7">
         <f>D60</f>
-        <v>42.5</v>
+        <v>11.25</v>
       </c>
       <c r="E63" s="7">
         <f>E60+C60-C63</f>
-        <v>36.084000000000003</v>
+        <v>18.042000000000002</v>
       </c>
       <c r="F63" s="7">
         <f>F60</f>
@@ -2256,42 +2400,166 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>112</v>
-      </c>
-      <c r="C64" s="7">
-        <f>C60</f>
-        <v>12.217000000000001</v>
+        <v>114</v>
+      </c>
+      <c r="C64" s="2">
+        <f>C63</f>
+        <v>77.168999999999997</v>
       </c>
       <c r="D64" s="7">
-        <v>61.25</v>
+        <f>D61</f>
+        <v>42.5</v>
       </c>
       <c r="E64" s="7">
-        <f>E63</f>
+        <f>E61+C61-C64</f>
         <v>36.084000000000003</v>
       </c>
       <c r="F64" s="7">
-        <f>F63</f>
+        <f>F61</f>
         <v>6.25</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C65" s="7">
-        <f>C59</f>
+        <f>C61</f>
+        <v>12.217000000000001</v>
+      </c>
+      <c r="D65" s="7">
+        <v>61.25</v>
+      </c>
+      <c r="E65" s="7">
+        <f>E64</f>
+        <v>36.084000000000003</v>
+      </c>
+      <c r="F65" s="7">
+        <f>F64</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>110</v>
+      </c>
+      <c r="C66" s="7">
+        <f>C60</f>
         <v>30.259</v>
       </c>
-      <c r="D65" s="7">
+      <c r="D66" s="7">
         <f>H26</f>
         <v>92.5</v>
       </c>
-      <c r="E65" s="7">
-        <f>E62</f>
+      <c r="E66" s="7">
+        <f>E63</f>
         <v>18.042000000000002</v>
       </c>
-      <c r="F65" s="7">
-        <f>F64</f>
+      <c r="F66" s="7">
+        <f>F65</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>116</v>
+      </c>
+      <c r="C68" s="2">
+        <f>C63</f>
+        <v>77.168999999999997</v>
+      </c>
+      <c r="D68" s="7">
+        <f>D14+D4-C8</f>
+        <v>23.75</v>
+      </c>
+      <c r="E68">
+        <f>ROUND(7/8*D6,3)</f>
+        <v>25.259</v>
+      </c>
+      <c r="F68" s="7">
+        <f>C8</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>118</v>
+      </c>
+      <c r="C69" s="2">
+        <f>C68-D6</f>
+        <v>48.301486540518709</v>
+      </c>
+      <c r="D69">
+        <f>D14+3*D4</f>
+        <v>80</v>
+      </c>
+      <c r="E69" s="7">
+        <f>ROUND(D6,3)</f>
+        <v>28.867999999999999</v>
+      </c>
+      <c r="F69" s="7">
+        <f>F68</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>117</v>
+      </c>
+      <c r="C70" s="2">
+        <f>C68</f>
+        <v>77.168999999999997</v>
+      </c>
+      <c r="D70">
+        <f>D14+3*D4</f>
+        <v>80</v>
+      </c>
+      <c r="E70">
+        <f>E68</f>
+        <v>25.259</v>
+      </c>
+      <c r="F70" s="7">
+        <f>F69</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>153</v>
+      </c>
+      <c r="C72">
+        <f>ROUND(C14+3.25*D6-C11-E72,3)</f>
+        <v>75.210999999999999</v>
+      </c>
+      <c r="D72" s="7">
+        <f>D66</f>
+        <v>92.5</v>
+      </c>
+      <c r="E72" s="12">
+        <v>20</v>
+      </c>
+      <c r="F72" s="7">
+        <f>F73</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>120</v>
+      </c>
+      <c r="C73" s="12">
+        <v>93.1</v>
+      </c>
+      <c r="D73" s="7">
+        <f>D68</f>
+        <v>23.75</v>
+      </c>
+      <c r="E73" s="2">
+        <f>C68+E68-C73</f>
+        <v>9.328000000000003</v>
+      </c>
+      <c r="F73" s="7">
+        <f>F68</f>
         <v>6.25</v>
       </c>
     </row>
@@ -2301,6 +2569,237 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AA91774-C951-4010-9B8F-40D8DBB1643F}">
+  <dimension ref="A4:F40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C11">
+        <v>0.2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>134</v>
+      </c>
+      <c r="C12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B14" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>126</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D17" t="s">
+        <v>128</v>
+      </c>
+      <c r="E17" t="s">
+        <v>129</v>
+      </c>
+      <c r="F17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>130</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="F21" s="13">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="F22" s="13">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>136</v>
+      </c>
+      <c r="C24" t="s">
+        <v>142</v>
+      </c>
+      <c r="D24" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>139</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="F25" s="13">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>137</v>
+      </c>
+      <c r="D26" s="13"/>
+      <c r="F26" s="13">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>138</v>
+      </c>
+      <c r="D27" s="13"/>
+      <c r="F27" s="13">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E28" s="13"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>147</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>148</v>
+      </c>
+      <c r="D36">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB32B072-E607-47EF-B931-ABD117479CC6}">
   <dimension ref="B2:AC79"/>
   <sheetViews>
@@ -3673,7 +4172,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7659A5BC-8263-4306-A02D-42C7263AD0FC}">
   <dimension ref="B2:U27"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update some tile groups with coloured tiles
</commit_message>
<xml_diff>
--- a/working/Geomorph Calcs.xlsx
+++ b/working/Geomorph Calcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\hextiles\working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695DEBE3-3DFB-4A00-AAF7-8A19642350B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B7B825-E0A3-4BB0-9D27-AB15A1277DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-14625" windowWidth="21600" windowHeight="11595" xr2:uid="{FF1B99F7-F5AF-49B6-8EDD-976A31B15329}"/>
+    <workbookView xWindow="22530" yWindow="-14535" windowWidth="21600" windowHeight="11595" activeTab="2" xr2:uid="{FF1B99F7-F5AF-49B6-8EDD-976A31B15329}"/>
   </bookViews>
   <sheets>
     <sheet name="Connections" sheetId="3" r:id="rId1"/>
@@ -956,7 +956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AA65B72-3617-498E-9A9E-6C122A9690F8}">
   <dimension ref="A2:AD76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+    <sheetView topLeftCell="A57" workbookViewId="0">
       <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
@@ -2887,8 +2887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB32B072-E607-47EF-B931-ABD117479CC6}">
   <dimension ref="B2:AC79"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>